<commit_message>
Futher work on docs
</commit_message>
<xml_diff>
--- a/DemoFiles/tvf_currencies.xlsx
+++ b/DemoFiles/tvf_currencies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python27\Scripts\querystorm-docs\docs\DemoFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9CD95504-79AE-4649-882D-E1BCC55CEF75}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{72A04C49-32E3-4BA3-A67D-166D4FA8007D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{1C823A0C-EE3B-4AD0-9F2A-1AB963C61E34}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Id</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>PLN</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Front wheel</t>
+  </si>
+  <si>
+    <t>Horn</t>
+  </si>
+  <si>
+    <t>Pedals</t>
   </si>
 </sst>
 </file>
@@ -103,7 +115,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -133,7 +149,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>800100</xdr:colOff>
+          <xdr:colOff>752475</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>123825</xdr:rowOff>
         </xdr:to>
@@ -184,11 +200,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{76EA2A48-8626-43D7-8B70-D32626E2694E}" name="Transactions" displayName="Transactions" ref="C3:G6" totalsRowShown="0">
-  <autoFilter ref="C3:G6" xr:uid="{CB68D97F-5EED-48A2-837C-4C120BA76B04}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{76EA2A48-8626-43D7-8B70-D32626E2694E}" name="Transactions" displayName="Transactions" ref="C3:H6" totalsRowShown="0">
+  <autoFilter ref="C3:H6" xr:uid="{CB68D97F-5EED-48A2-837C-4C120BA76B04}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{7025792A-1C64-45AA-A46F-809D19D800D1}" name="Id"/>
     <tableColumn id="5" xr3:uid="{C8ED9F75-4ECB-421A-8561-BA2E630E24FD}" name="Date"/>
+    <tableColumn id="6" xr3:uid="{DB6C33B9-9EB4-47AB-B09C-8CCCBDA34478}" name="Item" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{03650B58-EE59-4DA4-B2BC-AEECB324752B}" name="Amount"/>
     <tableColumn id="3" xr3:uid="{7E7391C6-3CDB-40D7-89FE-25274A313437}" name="Currency"/>
     <tableColumn id="4" xr3:uid="{6CE1E91C-A14D-433D-BAE4-55935EDDDB9D}" name="Target currencies"/>
@@ -495,18 +512,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC83C1CF-05DE-4ABE-9960-B29097ECADDF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="C3:O10"/>
+  <dimension ref="C3:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
@@ -514,7 +532,7 @@
     <col min="16" max="16" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -522,91 +540,103 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="4"/>
       <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
     </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" s="1">
         <v>43281</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4">
         <v>21.34</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="4"/>
       <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" s="1">
         <v>43237</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5">
         <v>88.12</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="4"/>
       <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" s="1">
         <v>43202</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6">
         <v>123.11</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>6</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="4"/>
       <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="J7" s="2"/>
       <c r="K7" s="3"/>
       <c r="L7" s="2"/>
@@ -614,7 +644,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="J8" s="2"/>
       <c r="K8" s="3"/>
       <c r="L8" s="2"/>
@@ -622,7 +652,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="J9" s="2"/>
       <c r="K9" s="3"/>
       <c r="L9" s="2"/>
@@ -630,7 +660,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="J10" s="2"/>
       <c r="K10" s="3"/>
       <c r="L10" s="2"/>
@@ -656,7 +686,7 @@
               </from>
               <to>
                 <xdr:col>5</xdr:col>
-                <xdr:colOff>800100</xdr:colOff>
+                <xdr:colOff>752475</xdr:colOff>
                 <xdr:row>9</xdr:row>
                 <xdr:rowOff>123825</xdr:rowOff>
               </to>
@@ -692,14 +722,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<Job xmlns="https://www.querystorm.com/automation" Name="Job 1" IsEnabled="true">
-  <Triggers xmlns="">
-    <Trigger Type="QueryStorm.Core.Triggers.ButtonTrigger">{"ButtonName":"Sheet1!CommandButton1"}</Trigger>
-  </Triggers>
-  <Actions xmlns="">
-    <Action Type="QueryStorm.Core.Automation.Actions.RunQueryAction">{"QueryId":"5333b18b-a771-4542-85bb-4e7210c854d6","Async":true}</Action>
-  </Actions>
-</Job>
+<EmbeddedQuery xmlns="www.querystorm.com/queries/files" Id="5333b18b-a771-4542-85bb-4e7210c854d6" FolderId="00000000-0000-0000-0000-000000000000" EngineConfig="SQLite ConnectionString='Data source=:memory:; DateTimeFormat=JulianDay' Scope='ActiveWorkbook'" Name="get results"><![CDATA[@Table TableName="result" DefaultAddress="Sheet1!J3"
+select
+	tr.Id, tr.Date, tr.Item, tr.Amount, tr.Currency as baseCurrency, ged.Currency as targetCurrency, round(Amount * Exchange, 2) as AmountInTargetCurrency
+from
+	Transactions tr,
+	GetExchangeData(tr.Date, tr.Currency, tr.[Target currencies]) ged  ]]></EmbeddedQuery>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -724,12 +752,14 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<EmbeddedQuery xmlns="www.querystorm.com/queries/files" Id="5333b18b-a771-4542-85bb-4e7210c854d6" FolderId="00000000-0000-0000-0000-000000000000" EngineConfig="SQLite ConnectionString='Data source=:memory:; DateTimeFormat=JulianDay' Scope='ActiveWorkbook'" Name="get results"><![CDATA[@Table TableName="result" DefaultAddress="Sheet1!J3"
-select
-	tr.Id, tr.Date, tr.Amount, tr.Currency as baseCurrency, ged.Currency as targetCurrency, round(Amount / Exchange, 2) as AmountInTargetCurrency
-from
-	Transactions tr,
-	GetExchangeData(tr.Date, tr.Currency, tr.[Target currencies]) ged  ]]></EmbeddedQuery>
+<Job xmlns="https://www.querystorm.com/automation" Name="Job 1" IsEnabled="true">
+  <Triggers xmlns="">
+    <Trigger Type="QueryStorm.Core.Triggers.ButtonTrigger">{"ButtonName":"Sheet1!CommandButton1"}</Trigger>
+  </Triggers>
+  <Actions xmlns="">
+    <Action Type="QueryStorm.Core.Automation.Actions.RunQueryAction">{"QueryId":"5333b18b-a771-4542-85bb-4e7210c854d6","Async":true}</Action>
+  </Actions>
+</Job>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -741,26 +771,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2342BEB-A3EE-4765-B7DB-F567231C87EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="www.querystorm.com/queries/files"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BB7A07-FD4B-45BD-9695-46CFD55FFBD4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="www.querystorm.com/queries/files"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACC39BC3-4FB0-4E0C-B9D6-4E93662B5514}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="https://www.querystorm.com/automation"/>
     <ds:schemaRef ds:uri=""/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BB7A07-FD4B-45BD-9695-46CFD55FFBD4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="www.querystorm.com/queries/files"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2342BEB-A3EE-4765-B7DB-F567231C87EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="www.querystorm.com/queries/files"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>